<commit_message>
Correción de CRUD Grilla DxDataGrid Datos Equipos y Caracteristicas
</commit_message>
<xml_diff>
--- a/ModeladorApp/wwwroot/uploads/MicroBase Equipos.xlsx
+++ b/ModeladorApp/wwwroot/uploads/MicroBase Equipos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\didie\Documents\Proyecto Modelador Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62BA7E6-824F-45F7-9FF0-032CD77AD8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEB1EE7-2DAD-4B53-950B-034A8067D5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{08961AB2-0B01-49D6-A199-DAAE7230915A}"/>
   </bookViews>
@@ -32,14 +32,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>EQUIPO</t>
   </si>
   <si>
-    <t>NCR</t>
-  </si>
-  <si>
     <t>EQUIPO ADMINISTRADOR DE ANCHO DE BANDA MARCA EXINDA modelo 3062-10</t>
   </si>
   <si>
@@ -80,13 +77,79 @@
   </si>
   <si>
     <t>Licencia de soporte premium para EXN-3062-36 Por 36 Meses</t>
+  </si>
+  <si>
+    <t>CANTIDAD</t>
+  </si>
+  <si>
+    <t>UNIDAD</t>
+  </si>
+  <si>
+    <t>DESCUENTO 1</t>
+  </si>
+  <si>
+    <t>SUBTOTAL 1</t>
+  </si>
+  <si>
+    <t>MRC</t>
+  </si>
+  <si>
+    <t>DESCUENTO 2</t>
+  </si>
+  <si>
+    <t>SUBTOTAL 2</t>
+  </si>
+  <si>
+    <t>UND</t>
+  </si>
+  <si>
+    <t>UND2</t>
+  </si>
+  <si>
+    <t>UND3</t>
+  </si>
+  <si>
+    <t>UND4</t>
+  </si>
+  <si>
+    <t>UND5</t>
+  </si>
+  <si>
+    <t>UND6</t>
+  </si>
+  <si>
+    <t>UND7</t>
+  </si>
+  <si>
+    <t>UND8</t>
+  </si>
+  <si>
+    <t>UND9</t>
+  </si>
+  <si>
+    <t>UND10</t>
+  </si>
+  <si>
+    <t>UND11</t>
+  </si>
+  <si>
+    <t>UND12</t>
+  </si>
+  <si>
+    <t>UND13</t>
+  </si>
+  <si>
+    <t>UND14</t>
+  </si>
+  <si>
+    <t>NRC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +161,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -445,138 +514,456 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{979C1FCF-924E-48E8-987D-C90390169BAD}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="78.77734375" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
       </c>
       <c r="B2" s="4">
         <v>1000</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2">
+        <v>10.15</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1500</v>
+      </c>
+      <c r="H2">
+        <v>10.15</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2">
         <v>120</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3">
+        <v>20.5</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>350</v>
+      </c>
+      <c r="H3">
+        <v>10.5</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2">
         <v>360</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4">
+        <v>20.5</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>200</v>
+      </c>
+      <c r="H4">
+        <v>10.5</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2">
         <v>420</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5">
+        <v>20.5</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>230</v>
+      </c>
+      <c r="H5">
+        <v>10.5</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6">
+        <v>20.5</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>210</v>
+      </c>
+      <c r="H6">
+        <v>10.5</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="2">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7">
+        <v>20.5</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>34</v>
+      </c>
+      <c r="H7">
+        <v>10.5</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="2">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8">
+        <v>20.5</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>50</v>
+      </c>
+      <c r="H8">
+        <v>10.5</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9">
+        <v>20.5</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>65</v>
+      </c>
+      <c r="H9">
+        <v>10.5</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="2">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10">
+        <v>20.5</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>85</v>
+      </c>
+      <c r="H10">
+        <v>10.5</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="2">
         <v>72</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11">
+        <v>20.5</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>96</v>
+      </c>
+      <c r="H11">
+        <v>10.5</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="4">
         <v>1200</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12">
+        <v>20.5</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1700</v>
+      </c>
+      <c r="H12">
+        <v>10.5</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2">
         <v>140</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13">
+        <v>20.5</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>150</v>
+      </c>
+      <c r="H13">
+        <v>10.5</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2">
         <v>244</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14">
+        <v>20.5</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>160</v>
+      </c>
+      <c r="H14">
+        <v>10.5</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2">
         <v>396</v>
       </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15">
+        <v>20.5</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>120</v>
+      </c>
+      <c r="H15">
+        <v>10.5</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>